<commit_message>
Modificat escalat del tst MN deñ insult service
</commit_message>
<xml_diff>
--- a/StressTests/RedisTests/single-node/resultats_tests.xlsx
+++ b/StressTests/RedisTests/single-node/resultats_tests.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Redis_Single_Filter" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Redis_Single_Service" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,6 +529,120 @@
         <v>300.27</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>InsultFilter</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Redis</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Single-node</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="G4" t="n">
+        <v>310.06</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Middleware</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Mode</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Clients</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Num Tasks</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Temps Total (s)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>RPS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>InsultService</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Redis</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Single-node</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="G2" t="n">
+        <v>950.27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>